<commit_message>
Added 2 test cases. 1. Login with valid credentials 2. Login with Invalid credentials
</commit_message>
<xml_diff>
--- a/src/test/resources/data/registerWithValid.xlsx
+++ b/src/test/resources/data/registerWithValid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zop9604/developer/git/Assignment/src/test/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D226089-E1AF-364A-9654-E304B7944D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA370026-14E4-0A40-8FC2-F51CAFE4C04B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2940" yWindow="2420" windowWidth="27640" windowHeight="16940" xr2:uid="{13B642A5-1081-D048-A0AD-915C3BD19931}"/>
   </bookViews>
@@ -436,7 +436,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>